<commit_message>
Correciones en la base
se cambió la base de datos, agregando el campo de fecha de impresión a
la llave primaria, para corregir el error al imprimir la lista de
facturas.
</commit_message>
<xml_diff>
--- a/Control de Reparto/Control de Reparto/Control de reparto.xlsx
+++ b/Control de Reparto/Control de Reparto/Control de reparto.xlsx
@@ -128,7 +128,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +148,14 @@
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -284,12 +292,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -319,15 +323,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -343,42 +386,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +688,7 @@
   <dimension ref="A1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -685,645 +697,632 @@
     <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.140625" customWidth="1"/>
+    <col min="12" max="12" width="36.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="18" t="s">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="32" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
     </row>
     <row r="3" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="35"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33" t="s">
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33" t="s">
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
     </row>
     <row r="7" spans="1:12">
-      <c r="A7" s="33"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="4" t="s">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="H7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="J7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="L7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="24" t="s">
+    <row r="8" spans="1:12" s="37" customFormat="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
     </row>
     <row r="9" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
     </row>
     <row r="10" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A10" s="26" t="s">
+      <c r="A10" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="27"/>
-      <c r="L10" s="28"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="18"/>
     </row>
     <row r="11" spans="1:12" ht="18.75" customHeight="1">
-      <c r="A11" s="29"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="30"/>
+      <c r="A11" s="19"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="18" t="s">
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="18" t="s">
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="18"/>
-      <c r="K13" s="18"/>
-      <c r="L13" s="10" t="s">
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:12" hidden="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
+      <c r="A14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="4.5" hidden="1" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
     </row>
     <row r="16" spans="1:12" hidden="1">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
-      <c r="L16" s="7"/>
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="1:12" hidden="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
     </row>
     <row r="18" spans="1:12">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18" t="s">
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="18" t="s">
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="18"/>
-      <c r="L18" s="10" t="s">
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-      <c r="K19" s="7"/>
-      <c r="L19" s="7"/>
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24" t="s">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23" t="s">
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23" t="s">
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
     </row>
     <row r="22" spans="1:12">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
+      <c r="A22" s="34"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16" t="s">
+      <c r="F23" s="28"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="16"/>
-      <c r="L23" s="16"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
     </row>
     <row r="24" spans="1:12" ht="7.5" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="21"/>
-      <c r="E25" s="21"/>
-      <c r="F25" s="21"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="22"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="33"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="19"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="30"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="7"/>
-      <c r="L29" s="7"/>
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="7"/>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="7"/>
-      <c r="K32" s="7"/>
-      <c r="L32" s="7"/>
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="7"/>
-      <c r="K33" s="7"/>
-      <c r="L33" s="7"/>
+      <c r="A33" s="5"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="7"/>
-      <c r="K34" s="7"/>
-      <c r="L34" s="7"/>
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="7"/>
-      <c r="K35" s="7"/>
-      <c r="L35" s="7"/>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="7"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="7"/>
-      <c r="K36" s="7"/>
-      <c r="L36" s="7"/>
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="7"/>
-      <c r="K37" s="7"/>
-      <c r="L37" s="7"/>
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="7"/>
-      <c r="G38" s="7"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="7"/>
-      <c r="K38" s="7"/>
-      <c r="L38" s="7"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="7"/>
-      <c r="H39" s="7"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="7"/>
-      <c r="K39" s="7"/>
-      <c r="L39" s="7"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A10:L11"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="J1:L1"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="C6:F7"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
     <mergeCell ref="J23:L23"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A25:L25"/>
@@ -1340,6 +1339,18 @@
     <mergeCell ref="E18:G18"/>
     <mergeCell ref="A23:D23"/>
     <mergeCell ref="E23:I23"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A10:L11"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="C6:F7"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>